<commit_message>
kind of works but not really
</commit_message>
<xml_diff>
--- a/Zeitplanen.xlsx
+++ b/Zeitplanen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Documents\GitHub\Project 335\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Documents\GitHub\modul152-Gallery-App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCE9246-AD71-4E85-8AA5-2D6EE06C417E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AED00FB-0F68-482C-8DE8-23D9CFF6AB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{4B305CFC-C0B3-4155-8BAF-9941DD21C0F0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Planen</t>
   </si>
@@ -113,13 +113,88 @@
   </si>
   <si>
     <t>1 </t>
+  </si>
+  <si>
+    <t>Farbe</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Hexadezimal</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>Solitude</t>
+  </si>
+  <si>
+    <t>#E5E7EB</t>
+  </si>
+  <si>
+    <t>229 231 235</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #ffffff</t>
+  </si>
+  <si>
+    <t>255 255 255</t>
+  </si>
+  <si>
+    <t>Slate Gray</t>
+  </si>
+  <si>
+    <t>#4B5563</t>
+  </si>
+  <si>
+    <t>75 85 99</t>
+  </si>
+  <si>
+    <t>Gainsboro</t>
+  </si>
+  <si>
+    <t>#D1D5DB</t>
+  </si>
+  <si>
+    <t>209 213 219</t>
+  </si>
+  <si>
+    <t>Cinnabar</t>
+  </si>
+  <si>
+    <t>#EF4444</t>
+  </si>
+  <si>
+    <t>239 68 68</t>
+  </si>
+  <si>
+    <t>Cornflower Blue</t>
+  </si>
+  <si>
+    <t>#3B82F6</t>
+  </si>
+  <si>
+    <t>59 130 246</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>0 0 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +274,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF2F5496"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,8 +336,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5E7EB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4B5563"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD1D5DB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEF4444"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3B82F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -441,11 +570,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -462,126 +643,156 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4B60CB-9A91-4A55-BDDC-A9937FEA8F07}">
-  <dimension ref="A1:AG38"/>
+  <dimension ref="A1:AN84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:K8"/>
+    <sheetView tabSelected="1" topLeftCell="X72" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AO83" sqref="AO83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,325 +1128,327 @@
     <col min="23" max="23" width="3.26953125" bestFit="1" customWidth="1"/>
     <col min="24" max="28" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="29" max="36" width="4" customWidth="1"/>
+    <col min="39" max="39" width="18.81640625" customWidth="1"/>
+    <col min="40" max="40" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A1" s="24"/>
-      <c r="B1" s="18">
+      <c r="A1" s="13"/>
+      <c r="B1" s="43">
         <v>44963</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43">
         <v>44964</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18">
+      <c r="E1" s="43"/>
+      <c r="F1" s="43">
         <v>44965</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43">
         <v>44966</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18">
+      <c r="I1" s="43"/>
+      <c r="J1" s="43">
         <v>44967</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="35">
+      <c r="K1" s="43"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="34">
         <v>44963</v>
       </c>
-      <c r="Y1" s="35">
+      <c r="Y1" s="34">
         <v>44964</v>
       </c>
-      <c r="Z1" s="35">
+      <c r="Z1" s="34">
         <v>44965</v>
       </c>
-      <c r="AA1" s="35">
+      <c r="AA1" s="34">
         <v>44966</v>
       </c>
-      <c r="AB1" s="35">
+      <c r="AB1" s="34">
         <v>44967</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="W2" s="30"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
     </row>
     <row r="3" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="22">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="11">
         <v>1</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="W3" s="31" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="W3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="X3" s="32">
+      <c r="X3" s="21">
         <v>0.5</v>
       </c>
-      <c r="Y3" s="32">
+      <c r="Y3" s="21">
         <v>0.5</v>
       </c>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="32"/>
-      <c r="AB3" s="32"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
     </row>
     <row r="4" spans="1:28" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="50">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25">
         <v>2</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="W4" s="20" t="s">
+      <c r="I4" s="25"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="W4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="37">
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28">
         <v>2</v>
       </c>
-      <c r="Z4" s="37">
+      <c r="Z4" s="28">
         <v>1</v>
       </c>
-      <c r="AA4" s="37">
+      <c r="AA4" s="28">
         <v>1</v>
       </c>
-      <c r="AB4" s="37">
+      <c r="AB4" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="23">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="12">
         <v>3</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="W5" s="21" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="W5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="38"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
     </row>
     <row r="6" spans="1:28" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="50">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25">
         <v>1</v>
       </c>
-      <c r="I6" s="50"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="W6" s="27" t="s">
+      <c r="I6" s="25"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="W6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="X6" s="39"/>
-      <c r="Y6" s="39">
+      <c r="X6" s="30"/>
+      <c r="Y6" s="30">
         <v>1</v>
       </c>
-      <c r="Z6" s="39"/>
-      <c r="AA6" s="39"/>
-      <c r="AB6" s="39"/>
+      <c r="Z6" s="30"/>
+      <c r="AA6" s="30"/>
+      <c r="AB6" s="30"/>
     </row>
     <row r="7" spans="1:28" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="47"/>
-      <c r="W7" s="28" t="s">
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="50"/>
+      <c r="W7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="X7" s="40"/>
-      <c r="Y7" s="40"/>
-      <c r="Z7" s="40"/>
-      <c r="AA7" s="40"/>
-      <c r="AB7" s="40"/>
+      <c r="X7" s="31"/>
+      <c r="Y7" s="31"/>
+      <c r="Z7" s="31"/>
+      <c r="AA7" s="31"/>
+      <c r="AB7" s="31"/>
     </row>
     <row r="8" spans="1:28" ht="84" x14ac:dyDescent="0.35">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="W8" s="20" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="W8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="37">
+      <c r="X8" s="36"/>
+      <c r="Y8" s="28">
         <v>2</v>
       </c>
-      <c r="Z8" s="37">
+      <c r="Z8" s="28">
         <v>2</v>
       </c>
-      <c r="AA8" s="37" t="s">
+      <c r="AA8" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="AB8" s="37"/>
+      <c r="AB8" s="28"/>
     </row>
     <row r="9" spans="1:28" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W9" s="21" t="s">
+      <c r="W9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="X9" s="42"/>
-      <c r="Y9" s="38"/>
-      <c r="Z9" s="38"/>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="29"/>
     </row>
     <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W10" s="29" t="s">
+      <c r="W10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="X10" s="33"/>
-      <c r="Y10" s="33"/>
-      <c r="Z10" s="34"/>
-      <c r="AA10" s="33">
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="23"/>
+      <c r="AA10" s="22">
         <v>3</v>
       </c>
-      <c r="AB10" s="33">
+      <c r="AB10" s="22">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="28" x14ac:dyDescent="0.35">
-      <c r="W11" s="20" t="s">
+      <c r="W11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="X11" s="37"/>
-      <c r="Y11" s="37">
+      <c r="X11" s="28"/>
+      <c r="Y11" s="28">
         <v>2</v>
       </c>
-      <c r="Z11" s="37">
+      <c r="Z11" s="28">
         <v>2</v>
       </c>
-      <c r="AA11" s="37"/>
-      <c r="AB11" s="37"/>
+      <c r="AA11" s="28"/>
+      <c r="AB11" s="28"/>
     </row>
     <row r="12" spans="1:28" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="W12" s="21" t="s">
+      <c r="W12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
-      <c r="Z12" s="38"/>
-      <c r="AA12" s="38"/>
-      <c r="AB12" s="38"/>
+      <c r="X12" s="29"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="29"/>
+      <c r="AB12" s="29"/>
     </row>
     <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L13" s="6"/>
-      <c r="W13" s="27" t="s">
+      <c r="W13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="X13" s="39"/>
-      <c r="Y13" s="43"/>
-      <c r="Z13" s="43"/>
-      <c r="AA13" s="39" t="s">
+      <c r="X13" s="30"/>
+      <c r="Y13" s="32"/>
+      <c r="Z13" s="32"/>
+      <c r="AA13" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="AB13" s="39" t="s">
+      <c r="AB13" s="30" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="L14" s="6"/>
-      <c r="W14" s="28" t="s">
+      <c r="W14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="X14" s="40"/>
-      <c r="Y14" s="44"/>
-      <c r="Z14" s="44"/>
-      <c r="AA14" s="40"/>
-      <c r="AB14" s="40"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="33"/>
+      <c r="Z14" s="33"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="31"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="L15" s="6"/>
@@ -1257,336 +1470,448 @@
     </row>
     <row r="21" spans="12:33" x14ac:dyDescent="0.35">
       <c r="W21" s="1"/>
-      <c r="X21" s="8">
+      <c r="X21" s="44">
         <v>44963</v>
       </c>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="8">
+      <c r="Y21" s="44"/>
+      <c r="Z21" s="44">
         <v>44964</v>
       </c>
-      <c r="AA21" s="8"/>
-      <c r="AB21" s="8">
+      <c r="AA21" s="44"/>
+      <c r="AB21" s="44">
         <v>44965</v>
       </c>
-      <c r="AC21" s="8"/>
-      <c r="AD21" s="8">
+      <c r="AC21" s="44"/>
+      <c r="AD21" s="44">
         <v>44966</v>
       </c>
-      <c r="AE21" s="8"/>
-      <c r="AF21" s="8">
+      <c r="AE21" s="44"/>
+      <c r="AF21" s="44">
         <v>44967</v>
       </c>
-      <c r="AG21" s="8"/>
+      <c r="AG21" s="44"/>
     </row>
     <row r="22" spans="12:33" x14ac:dyDescent="0.35">
       <c r="W22" s="1"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
-      <c r="AC22" s="9"/>
-      <c r="AD22" s="9"/>
-      <c r="AE22" s="9"/>
-      <c r="AF22" s="9"/>
-      <c r="AG22" s="9"/>
+      <c r="X22" s="45"/>
+      <c r="Y22" s="45"/>
+      <c r="Z22" s="45"/>
+      <c r="AA22" s="45"/>
+      <c r="AB22" s="45"/>
+      <c r="AC22" s="45"/>
+      <c r="AD22" s="45"/>
+      <c r="AE22" s="45"/>
+      <c r="AF22" s="45"/>
+      <c r="AG22" s="45"/>
     </row>
     <row r="23" spans="12:33" x14ac:dyDescent="0.35">
       <c r="W23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="X23" s="16">
+      <c r="X23" s="39">
         <v>0.5</v>
       </c>
-      <c r="Y23" s="17"/>
-      <c r="Z23" s="16">
+      <c r="Y23" s="40"/>
+      <c r="Z23" s="39">
         <v>0.5</v>
       </c>
-      <c r="AA23" s="17"/>
-      <c r="AB23" s="16"/>
-      <c r="AC23" s="17"/>
-      <c r="AD23" s="16"/>
-      <c r="AE23" s="17"/>
-      <c r="AF23" s="16"/>
-      <c r="AG23" s="17"/>
+      <c r="AA23" s="40"/>
+      <c r="AB23" s="39"/>
+      <c r="AC23" s="40"/>
+      <c r="AD23" s="39"/>
+      <c r="AE23" s="40"/>
+      <c r="AF23" s="39"/>
+      <c r="AG23" s="40"/>
     </row>
     <row r="24" spans="12:33" ht="174" x14ac:dyDescent="0.35">
       <c r="W24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="17"/>
-      <c r="Z24" s="16">
+      <c r="X24" s="39"/>
+      <c r="Y24" s="40"/>
+      <c r="Z24" s="39">
         <v>1</v>
       </c>
-      <c r="AA24" s="17"/>
-      <c r="AB24" s="16">
+      <c r="AA24" s="40"/>
+      <c r="AB24" s="39">
         <v>1</v>
       </c>
-      <c r="AC24" s="17"/>
-      <c r="AD24" s="16">
+      <c r="AC24" s="40"/>
+      <c r="AD24" s="39">
         <v>1</v>
       </c>
-      <c r="AE24" s="17"/>
-      <c r="AF24" s="16">
+      <c r="AE24" s="40"/>
+      <c r="AF24" s="39">
         <v>1</v>
       </c>
-      <c r="AG24" s="17"/>
+      <c r="AG24" s="40"/>
     </row>
     <row r="25" spans="12:33" ht="101.5" x14ac:dyDescent="0.35">
       <c r="W25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="15"/>
-      <c r="Z25" s="14">
+      <c r="X25" s="26"/>
+      <c r="Y25" s="38"/>
+      <c r="Z25" s="26">
         <v>1</v>
       </c>
-      <c r="AA25" s="15"/>
-      <c r="AB25" s="14"/>
-      <c r="AC25" s="15"/>
-      <c r="AD25" s="14"/>
-      <c r="AE25" s="15"/>
-      <c r="AF25" s="14"/>
-      <c r="AG25" s="15"/>
+      <c r="AA25" s="38"/>
+      <c r="AB25" s="26"/>
+      <c r="AC25" s="38"/>
+      <c r="AD25" s="26"/>
+      <c r="AE25" s="38"/>
+      <c r="AF25" s="26"/>
+      <c r="AG25" s="38"/>
     </row>
     <row r="26" spans="12:33" ht="130.5" x14ac:dyDescent="0.35">
       <c r="W26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="X26" s="16">
+      <c r="X26" s="39">
         <v>2</v>
       </c>
-      <c r="Y26" s="17"/>
-      <c r="Z26" s="16">
+      <c r="Y26" s="40"/>
+      <c r="Z26" s="39">
         <v>2</v>
       </c>
-      <c r="AA26" s="17"/>
-      <c r="AB26" s="16">
+      <c r="AA26" s="40"/>
+      <c r="AB26" s="39">
         <v>2</v>
       </c>
-      <c r="AC26" s="17"/>
-      <c r="AD26" s="16"/>
-      <c r="AE26" s="17"/>
-      <c r="AF26" s="16"/>
-      <c r="AG26" s="17"/>
+      <c r="AC26" s="40"/>
+      <c r="AD26" s="39"/>
+      <c r="AE26" s="40"/>
+      <c r="AF26" s="39"/>
+      <c r="AG26" s="40"/>
     </row>
     <row r="27" spans="12:33" x14ac:dyDescent="0.35">
       <c r="W27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="15"/>
-      <c r="AB27" s="14">
+      <c r="X27" s="26"/>
+      <c r="Y27" s="38"/>
+      <c r="Z27" s="26"/>
+      <c r="AA27" s="38"/>
+      <c r="AB27" s="26">
         <v>3</v>
       </c>
-      <c r="AC27" s="15"/>
-      <c r="AD27" s="14"/>
-      <c r="AE27" s="15"/>
-      <c r="AF27" s="14"/>
-      <c r="AG27" s="15"/>
+      <c r="AC27" s="38"/>
+      <c r="AD27" s="26"/>
+      <c r="AE27" s="38"/>
+      <c r="AF27" s="26"/>
+      <c r="AG27" s="38"/>
     </row>
     <row r="28" spans="12:33" ht="87" x14ac:dyDescent="0.35">
       <c r="W28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="X28" s="16"/>
-      <c r="Y28" s="17"/>
-      <c r="Z28" s="16">
+      <c r="X28" s="39"/>
+      <c r="Y28" s="40"/>
+      <c r="Z28" s="39">
         <v>2</v>
       </c>
-      <c r="AA28" s="17"/>
-      <c r="AB28" s="16">
+      <c r="AA28" s="40"/>
+      <c r="AB28" s="39">
         <v>2</v>
       </c>
-      <c r="AC28" s="17"/>
-      <c r="AD28" s="16"/>
-      <c r="AE28" s="17"/>
-      <c r="AF28" s="16"/>
-      <c r="AG28" s="17"/>
+      <c r="AC28" s="40"/>
+      <c r="AD28" s="39"/>
+      <c r="AE28" s="40"/>
+      <c r="AF28" s="39"/>
+      <c r="AG28" s="40"/>
     </row>
     <row r="29" spans="12:33" ht="116" x14ac:dyDescent="0.35">
       <c r="W29" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="15"/>
-      <c r="Z29" s="14">
+      <c r="X29" s="26"/>
+      <c r="Y29" s="38"/>
+      <c r="Z29" s="26">
         <v>1</v>
       </c>
-      <c r="AA29" s="15"/>
-      <c r="AB29" s="14">
+      <c r="AA29" s="38"/>
+      <c r="AB29" s="26">
         <v>1</v>
       </c>
-      <c r="AC29" s="15"/>
-      <c r="AD29" s="14"/>
-      <c r="AE29" s="15"/>
-      <c r="AF29" s="14"/>
-      <c r="AG29" s="15"/>
+      <c r="AC29" s="38"/>
+      <c r="AD29" s="26"/>
+      <c r="AE29" s="38"/>
+      <c r="AF29" s="26"/>
+      <c r="AG29" s="38"/>
     </row>
     <row r="30" spans="12:33" x14ac:dyDescent="0.35">
       <c r="W30" s="2"/>
-      <c r="X30" s="10"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="10"/>
-      <c r="AA30" s="11"/>
-      <c r="AB30" s="10"/>
-      <c r="AC30" s="11"/>
-      <c r="AD30" s="10"/>
-      <c r="AE30" s="11"/>
-      <c r="AF30" s="10"/>
-      <c r="AG30" s="11"/>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="42"/>
+      <c r="Z30" s="41"/>
+      <c r="AA30" s="42"/>
+      <c r="AB30" s="41"/>
+      <c r="AC30" s="42"/>
+      <c r="AD30" s="41"/>
+      <c r="AE30" s="42"/>
+      <c r="AF30" s="41"/>
+      <c r="AG30" s="42"/>
     </row>
     <row r="31" spans="12:33" x14ac:dyDescent="0.35">
       <c r="W31" s="3"/>
-      <c r="X31" s="10"/>
-      <c r="Y31" s="11"/>
-      <c r="Z31" s="10"/>
-      <c r="AA31" s="11"/>
-      <c r="AB31" s="10"/>
-      <c r="AC31" s="11"/>
-      <c r="AD31" s="10"/>
-      <c r="AE31" s="11"/>
-      <c r="AF31" s="10"/>
-      <c r="AG31" s="11"/>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="42"/>
+      <c r="Z31" s="41"/>
+      <c r="AA31" s="42"/>
+      <c r="AB31" s="41"/>
+      <c r="AC31" s="42"/>
+      <c r="AD31" s="41"/>
+      <c r="AE31" s="42"/>
+      <c r="AF31" s="41"/>
+      <c r="AG31" s="42"/>
     </row>
     <row r="32" spans="12:33" x14ac:dyDescent="0.35">
       <c r="W32" s="2"/>
-      <c r="X32" s="12"/>
-      <c r="Y32" s="13"/>
-      <c r="Z32" s="12"/>
-      <c r="AA32" s="13"/>
-      <c r="AB32" s="12"/>
-      <c r="AC32" s="13"/>
-      <c r="AD32" s="12"/>
-      <c r="AE32" s="13"/>
-      <c r="AF32" s="12"/>
-      <c r="AG32" s="13"/>
+      <c r="X32" s="46"/>
+      <c r="Y32" s="47"/>
+      <c r="Z32" s="46"/>
+      <c r="AA32" s="47"/>
+      <c r="AB32" s="46"/>
+      <c r="AC32" s="47"/>
+      <c r="AD32" s="46"/>
+      <c r="AE32" s="47"/>
+      <c r="AF32" s="46"/>
+      <c r="AG32" s="47"/>
     </row>
     <row r="33" spans="23:33" x14ac:dyDescent="0.35">
       <c r="W33" s="3"/>
-      <c r="X33" s="10"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="10"/>
-      <c r="AA33" s="11"/>
-      <c r="AB33" s="10"/>
-      <c r="AC33" s="11"/>
-      <c r="AD33" s="10"/>
-      <c r="AE33" s="11"/>
-      <c r="AF33" s="10"/>
-      <c r="AG33" s="11"/>
+      <c r="X33" s="41"/>
+      <c r="Y33" s="42"/>
+      <c r="Z33" s="41"/>
+      <c r="AA33" s="42"/>
+      <c r="AB33" s="41"/>
+      <c r="AC33" s="42"/>
+      <c r="AD33" s="41"/>
+      <c r="AE33" s="42"/>
+      <c r="AF33" s="41"/>
+      <c r="AG33" s="42"/>
     </row>
     <row r="34" spans="23:33" x14ac:dyDescent="0.35">
       <c r="W34" s="2"/>
-      <c r="X34" s="12"/>
-      <c r="Y34" s="13"/>
-      <c r="Z34" s="12"/>
-      <c r="AA34" s="13"/>
-      <c r="AB34" s="12"/>
-      <c r="AC34" s="13"/>
-      <c r="AD34" s="12"/>
-      <c r="AE34" s="13"/>
-      <c r="AF34" s="12"/>
-      <c r="AG34" s="13"/>
+      <c r="X34" s="46"/>
+      <c r="Y34" s="47"/>
+      <c r="Z34" s="46"/>
+      <c r="AA34" s="47"/>
+      <c r="AB34" s="46"/>
+      <c r="AC34" s="47"/>
+      <c r="AD34" s="46"/>
+      <c r="AE34" s="47"/>
+      <c r="AF34" s="46"/>
+      <c r="AG34" s="47"/>
     </row>
     <row r="35" spans="23:33" x14ac:dyDescent="0.35">
       <c r="W35" s="3"/>
-      <c r="X35" s="10"/>
-      <c r="Y35" s="11"/>
-      <c r="Z35" s="10"/>
-      <c r="AA35" s="11"/>
-      <c r="AB35" s="10"/>
-      <c r="AC35" s="11"/>
-      <c r="AD35" s="10"/>
-      <c r="AE35" s="11"/>
-      <c r="AF35" s="10"/>
-      <c r="AG35" s="11"/>
+      <c r="X35" s="41"/>
+      <c r="Y35" s="42"/>
+      <c r="Z35" s="41"/>
+      <c r="AA35" s="42"/>
+      <c r="AB35" s="41"/>
+      <c r="AC35" s="42"/>
+      <c r="AD35" s="41"/>
+      <c r="AE35" s="42"/>
+      <c r="AF35" s="41"/>
+      <c r="AG35" s="42"/>
     </row>
     <row r="36" spans="23:33" x14ac:dyDescent="0.35">
       <c r="W36" s="2"/>
-      <c r="X36" s="12"/>
-      <c r="Y36" s="13"/>
-      <c r="Z36" s="12"/>
-      <c r="AA36" s="13"/>
-      <c r="AB36" s="12"/>
-      <c r="AC36" s="13"/>
-      <c r="AD36" s="12"/>
-      <c r="AE36" s="13"/>
-      <c r="AF36" s="12"/>
-      <c r="AG36" s="13"/>
+      <c r="X36" s="46"/>
+      <c r="Y36" s="47"/>
+      <c r="Z36" s="46"/>
+      <c r="AA36" s="47"/>
+      <c r="AB36" s="46"/>
+      <c r="AC36" s="47"/>
+      <c r="AD36" s="46"/>
+      <c r="AE36" s="47"/>
+      <c r="AF36" s="46"/>
+      <c r="AG36" s="47"/>
     </row>
     <row r="37" spans="23:33" x14ac:dyDescent="0.35">
       <c r="W37" s="3"/>
-      <c r="X37" s="10"/>
-      <c r="Y37" s="11"/>
-      <c r="Z37" s="10"/>
-      <c r="AA37" s="11"/>
-      <c r="AB37" s="10"/>
-      <c r="AC37" s="11"/>
-      <c r="AD37" s="10"/>
-      <c r="AE37" s="11"/>
-      <c r="AF37" s="10"/>
-      <c r="AG37" s="11"/>
+      <c r="X37" s="41"/>
+      <c r="Y37" s="42"/>
+      <c r="Z37" s="41"/>
+      <c r="AA37" s="42"/>
+      <c r="AB37" s="41"/>
+      <c r="AC37" s="42"/>
+      <c r="AD37" s="41"/>
+      <c r="AE37" s="42"/>
+      <c r="AF37" s="41"/>
+      <c r="AG37" s="42"/>
     </row>
     <row r="38" spans="23:33" x14ac:dyDescent="0.35">
       <c r="W38" s="2"/>
-      <c r="X38" s="12"/>
-      <c r="Y38" s="13"/>
-      <c r="Z38" s="12"/>
-      <c r="AA38" s="13"/>
-      <c r="AB38" s="12"/>
-      <c r="AC38" s="13"/>
-      <c r="AD38" s="12"/>
-      <c r="AE38" s="13"/>
-      <c r="AF38" s="12"/>
-      <c r="AG38" s="13"/>
+      <c r="X38" s="46"/>
+      <c r="Y38" s="47"/>
+      <c r="Z38" s="46"/>
+      <c r="AA38" s="47"/>
+      <c r="AB38" s="46"/>
+      <c r="AC38" s="47"/>
+      <c r="AD38" s="46"/>
+      <c r="AE38" s="47"/>
+      <c r="AF38" s="46"/>
+      <c r="AG38" s="47"/>
+    </row>
+    <row r="76" spans="37:40" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="77" spans="37:40" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK77" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL77" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM77" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN77" s="52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="37:40" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK78" s="55"/>
+      <c r="AL78" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM78" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN78" s="54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="37:40" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK79" s="53"/>
+      <c r="AL79" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM79" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN79" s="54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="37:40" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK80" s="57"/>
+      <c r="AL80" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM80" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN80" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="37:40" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK81" s="59"/>
+      <c r="AL81" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM81" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN81" s="54" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="82" spans="37:40" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK82" s="58"/>
+      <c r="AL82" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM82" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN82" s="54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="37:40" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK83" s="56"/>
+      <c r="AL83" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM83" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN83" s="54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="37:40" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK84" s="60"/>
+      <c r="AL84" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM84" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN84" s="54" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="122">
-    <mergeCell ref="B8:K8"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="AA8:AA9"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="Y11:Y12"/>
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="AA11:AA12"/>
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="Y4:Y5"/>
-    <mergeCell ref="Z4:Z5"/>
-    <mergeCell ref="AA4:AA5"/>
-    <mergeCell ref="AB4:AB5"/>
-    <mergeCell ref="X6:X7"/>
-    <mergeCell ref="Y6:Y7"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AB6:AB7"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="X8:X9"/>
-    <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="X29:Y29"/>
-    <mergeCell ref="X30:Y30"/>
-    <mergeCell ref="X31:Y31"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="X21:Y22"/>
+    <mergeCell ref="Z21:AA22"/>
+    <mergeCell ref="Z37:AA37"/>
+    <mergeCell ref="Z38:AA38"/>
+    <mergeCell ref="AF21:AG22"/>
+    <mergeCell ref="AD21:AE22"/>
+    <mergeCell ref="AB21:AC22"/>
+    <mergeCell ref="Z32:AA32"/>
+    <mergeCell ref="Z33:AA33"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="Z35:AA35"/>
+    <mergeCell ref="Z36:AA36"/>
+    <mergeCell ref="Z27:AA27"/>
+    <mergeCell ref="Z28:AA28"/>
+    <mergeCell ref="Z29:AA29"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="Z31:AA31"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="Z26:AA26"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="AB35:AC35"/>
+    <mergeCell ref="AB36:AC36"/>
+    <mergeCell ref="AB37:AC37"/>
+    <mergeCell ref="AB38:AC38"/>
+    <mergeCell ref="AD35:AE35"/>
+    <mergeCell ref="AD36:AE36"/>
+    <mergeCell ref="AD37:AE37"/>
+    <mergeCell ref="AD38:AE38"/>
+    <mergeCell ref="AB23:AC23"/>
+    <mergeCell ref="AB24:AC24"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="AB27:AC27"/>
+    <mergeCell ref="AB28:AC28"/>
+    <mergeCell ref="AB29:AC29"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AB32:AC32"/>
+    <mergeCell ref="AB33:AC33"/>
+    <mergeCell ref="AF36:AG36"/>
+    <mergeCell ref="AF37:AG37"/>
+    <mergeCell ref="AF38:AG38"/>
+    <mergeCell ref="AD23:AE23"/>
+    <mergeCell ref="AD24:AE24"/>
+    <mergeCell ref="AD25:AE25"/>
+    <mergeCell ref="AD26:AE26"/>
+    <mergeCell ref="AD27:AE27"/>
+    <mergeCell ref="AD28:AE28"/>
+    <mergeCell ref="AD29:AE29"/>
+    <mergeCell ref="AD30:AE30"/>
+    <mergeCell ref="AD31:AE31"/>
+    <mergeCell ref="AD32:AE32"/>
+    <mergeCell ref="AD33:AE33"/>
+    <mergeCell ref="AD34:AE34"/>
     <mergeCell ref="X37:Y37"/>
     <mergeCell ref="X38:Y38"/>
     <mergeCell ref="AF23:AG23"/>
@@ -1611,62 +1936,49 @@
     <mergeCell ref="X24:Y24"/>
     <mergeCell ref="X25:Y25"/>
     <mergeCell ref="X26:Y26"/>
-    <mergeCell ref="AF36:AG36"/>
-    <mergeCell ref="AF37:AG37"/>
-    <mergeCell ref="AF38:AG38"/>
-    <mergeCell ref="AD23:AE23"/>
-    <mergeCell ref="AD24:AE24"/>
-    <mergeCell ref="AD25:AE25"/>
-    <mergeCell ref="AD26:AE26"/>
-    <mergeCell ref="AD27:AE27"/>
-    <mergeCell ref="AD28:AE28"/>
-    <mergeCell ref="AD29:AE29"/>
-    <mergeCell ref="AD30:AE30"/>
-    <mergeCell ref="AD31:AE31"/>
-    <mergeCell ref="AD32:AE32"/>
-    <mergeCell ref="AD33:AE33"/>
-    <mergeCell ref="AD34:AE34"/>
-    <mergeCell ref="AB38:AC38"/>
-    <mergeCell ref="AD35:AE35"/>
-    <mergeCell ref="AD36:AE36"/>
-    <mergeCell ref="AD37:AE37"/>
-    <mergeCell ref="AD38:AE38"/>
-    <mergeCell ref="AB23:AC23"/>
-    <mergeCell ref="AB24:AC24"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AB26:AC26"/>
-    <mergeCell ref="AB27:AC27"/>
-    <mergeCell ref="AB28:AC28"/>
-    <mergeCell ref="AB29:AC29"/>
-    <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="AB31:AC31"/>
-    <mergeCell ref="AB32:AC32"/>
-    <mergeCell ref="AB33:AC33"/>
-    <mergeCell ref="Z21:AA22"/>
-    <mergeCell ref="Z37:AA37"/>
-    <mergeCell ref="Z38:AA38"/>
-    <mergeCell ref="AF21:AG22"/>
-    <mergeCell ref="AD21:AE22"/>
-    <mergeCell ref="AB21:AC22"/>
-    <mergeCell ref="Z32:AA32"/>
-    <mergeCell ref="Z33:AA33"/>
-    <mergeCell ref="Z34:AA34"/>
-    <mergeCell ref="Z35:AA35"/>
-    <mergeCell ref="Z36:AA36"/>
-    <mergeCell ref="Z27:AA27"/>
-    <mergeCell ref="Z28:AA28"/>
-    <mergeCell ref="Z29:AA29"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="Z31:AA31"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="Z26:AA26"/>
-    <mergeCell ref="AB34:AC34"/>
-    <mergeCell ref="AB35:AC35"/>
-    <mergeCell ref="AB36:AC36"/>
-    <mergeCell ref="AB37:AC37"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="X29:Y29"/>
+    <mergeCell ref="X30:Y30"/>
+    <mergeCell ref="X31:Y31"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="X21:Y22"/>
     <mergeCell ref="B7:K7"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="X4:X5"/>
+    <mergeCell ref="Y4:Y5"/>
+    <mergeCell ref="Z4:Z5"/>
+    <mergeCell ref="AA4:AA5"/>
+    <mergeCell ref="AB4:AB5"/>
+    <mergeCell ref="X6:X7"/>
+    <mergeCell ref="Y6:Y7"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="AB6:AB7"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="AA8:AA9"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AB11:AB12"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>